<commit_message>
Better u16 divP & modP
Improved the unsigned 16-bit precomputed division/modulo methods:
- Calculating the precomputed divisors now only needs a single 16-bit division (>2x faster!)
- Changed `divMagic` struct members to: reciprocal + divisors vecs
- New division method: similar speed
- New modulo method: 2-4 fewer instructions (perf +20%?)
- Modulo P ABI change: no divisors argument as magic struct already contains them (method always needs to calculate the remainder)
- Updated performance test & excel results to reflect these changes

Additional:
- Fixed sat. conversion typo (u64x4 => u64x2)
- Better `perfDivByScalar` type specifier ("%llu" => "%zu")
</commit_message>
<xml_diff>
--- a/external/PerfDivByScalar.xlsx
+++ b/external/PerfDivByScalar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walte\Desktop\Coding\Filling SIMD gaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8AC2C3-BD0B-4C60-913E-1979CE70D456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5C83B9-5201-49EB-95A4-F3655FE5D934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{395B90C2-E5A1-4B1B-8B08-7B8CE154B6A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{395B90C2-E5A1-4B1B-8B08-7B8CE154B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Div 8-bit</t>
   </si>
@@ -178,12 +178,35 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>Approx curret ver</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ryzen 8400f 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Zen4)</t>
+    </r>
+  </si>
+  <si>
+    <t>Red is old ver</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +252,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97F82"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,6 +529,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,9 +584,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF97F82"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FFFF5D5D"/>
-      <color rgb="FFF97F82"/>
     </mruColors>
   </colors>
   <extLst>
@@ -860,23 +917,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0081CB9-D5CB-4347-8A8C-5099AF4A23F5}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="3" max="7" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="3" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
@@ -884,34 +941,38 @@
         <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
-      <c r="I2" s="17" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="J2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -922,20 +983,23 @@
         <v>2.06</v>
       </c>
       <c r="E3" s="8">
+        <v>1.77</v>
+      </c>
+      <c r="F3" s="8">
         <v>13.01</v>
       </c>
-      <c r="F3" s="8">
+      <c r="G3" s="8">
         <v>4.0599999999999996</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>5.45</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -946,16 +1010,19 @@
         <v>0.71</v>
       </c>
       <c r="E4" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="F4" s="8">
         <v>4.88</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="8">
         <v>1.68</v>
       </c>
-      <c r="G4" s="12">
+      <c r="H4" s="12">
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
@@ -968,30 +1035,35 @@
         <v>1.9014084507042255</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" ref="E5:G5" si="0">(E3-E4)/E4</f>
+        <f>(E3-E4)/E4</f>
+        <v>1.7656249999999998</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" ref="F5:H5" si="0">(F3-F4)/F4</f>
         <v>1.665983606557377</v>
       </c>
-      <c r="F5" s="8">
+      <c r="G5" s="8">
         <f t="shared" si="0"/>
         <v>1.4166666666666667</v>
       </c>
-      <c r="G5" s="12">
+      <c r="H5" s="12">
         <f t="shared" si="0"/>
         <v>3.7807017543859658</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1002,92 +1074,131 @@
         <v>0.82</v>
       </c>
       <c r="E7" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="8">
         <v>7.18</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <v>1.99</v>
       </c>
-      <c r="G7" s="12">
+      <c r="H7" s="12">
         <v>2.67</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="19">
         <v>0.8</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="19">
         <v>0.81</v>
       </c>
       <c r="E8" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="F8" s="19">
         <v>5.16</v>
       </c>
-      <c r="F8" s="8">
-        <v>2.38</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="G8" s="21">
+        <v>1.82</v>
+      </c>
+      <c r="H8" s="20">
         <v>2.36</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="19">
         <f>(C7-C8)/C8</f>
         <v>-0.12500000000000011</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="19">
         <f>(D7-D8)/D8</f>
         <v>1.2345679012345552E-2</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" ref="E9" si="1">(E7-E8)/E8</f>
+        <f>(E7-E8)/E8</f>
+        <v>9.3749999999999903E-2</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" ref="F9" si="1">(F7-F8)/F8</f>
         <v>0.39147286821705418</v>
       </c>
-      <c r="F9" s="8">
-        <f t="shared" ref="F9:G9" si="2">(F7-F8)/F8</f>
-        <v>-0.16386554621848737</v>
-      </c>
-      <c r="G9" s="12">
+      <c r="G9" s="21">
+        <f t="shared" ref="G9:H9" si="2">(G7-G8)/G8</f>
+        <v>9.3406593406593366E-2</v>
+      </c>
+      <c r="H9" s="20">
         <f t="shared" si="2"/>
         <v>0.13135593220338987</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="8">
+        <f>J11*0.8</f>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" ref="D11:H11" si="3">J11*0.8</f>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="3"/>
+        <v>6.5680000000000014</v>
+      </c>
+      <c r="G11" s="8">
+        <v>3.95</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="3"/>
+        <v>3.5200000000000005</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="8">
         <v>1.17</v>
       </c>
-      <c r="D11" s="8">
+      <c r="K11" s="8">
         <v>1.33</v>
       </c>
-      <c r="E11" s="8">
+      <c r="L11" s="8">
         <v>8.2100000000000009</v>
       </c>
-      <c r="F11" s="8">
+      <c r="M11" s="8">
         <v>3.97</v>
       </c>
-      <c r="G11" s="12">
+      <c r="N11" s="12">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1098,52 +1209,60 @@
         <v>0.93</v>
       </c>
       <c r="E12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="8">
         <v>7.01</v>
       </c>
-      <c r="F12" s="8">
-        <v>4.4400000000000004</v>
-      </c>
-      <c r="G12" s="12">
+      <c r="G12" s="8">
+        <v>4.42</v>
+      </c>
+      <c r="H12" s="12">
         <v>3.66</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="8">
         <f>(C11-C12)/C12</f>
-        <v>4.4642857142856977E-2</v>
+        <v>-0.16428571428571442</v>
       </c>
       <c r="D13" s="8">
         <f>(D11-D12)/D12</f>
-        <v>0.43010752688172044</v>
+        <v>6.4516129032256928E-3</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" ref="E13" si="3">(E11-E12)/E12</f>
-        <v>0.17118402282453654</v>
+        <f>(E11-E12)/E12</f>
+        <v>0.21249999999999991</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" ref="F13:G13" si="4">(F11-F12)/F12</f>
-        <v>-0.10585585585585588</v>
-      </c>
-      <c r="G13" s="12">
-        <f t="shared" si="4"/>
-        <v>0.20218579234972683</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+        <f t="shared" ref="F13" si="4">(F11-F12)/F12</f>
+        <v>-6.305278174037067E-2</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" ref="G13:H13" si="5">(G11-G12)/G12</f>
+        <v>-0.10633484162895922</v>
+      </c>
+      <c r="H13" s="12">
+        <f t="shared" si="5"/>
+        <v>-3.825136612021849E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>1</v>
@@ -1155,54 +1274,61 @@
         <v>1.67</v>
       </c>
       <c r="E15" s="11">
+        <v>1.48</v>
+      </c>
+      <c r="F15" s="11">
         <v>7.6</v>
       </c>
-      <c r="F15" s="11">
-        <v>7.79</v>
-      </c>
-      <c r="G15" s="13">
+      <c r="G15" s="11">
+        <v>6.55</v>
+      </c>
+      <c r="H15" s="13">
         <v>1.69</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="8"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4" t="s">
         <v>1</v>
@@ -1214,16 +1340,19 @@
         <v>2.62</v>
       </c>
       <c r="E20" s="8">
+        <v>2.04</v>
+      </c>
+      <c r="F20" s="8">
         <v>14.88</v>
       </c>
-      <c r="F20" s="8">
+      <c r="G20" s="8">
         <v>4.1500000000000004</v>
       </c>
-      <c r="G20" s="12">
+      <c r="H20" s="12">
         <v>5.42</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1234,16 +1363,19 @@
         <v>0.72</v>
       </c>
       <c r="E21" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="F21" s="8">
         <v>4.46</v>
       </c>
-      <c r="F21" s="8">
+      <c r="G21" s="8">
         <v>2.13</v>
       </c>
-      <c r="G21" s="12">
+      <c r="H21" s="12">
         <v>1.32</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1256,30 +1388,35 @@
         <v>2.6388888888888893</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" ref="E22" si="5">(E20-E21)/E21</f>
+        <f>(E20-E21)/E21</f>
+        <v>2.0909090909090908</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" ref="F22" si="6">(F20-F21)/F21</f>
         <v>2.3363228699551573</v>
       </c>
-      <c r="F22" s="8">
-        <f t="shared" ref="F22:G22" si="6">(F20-F21)/F21</f>
+      <c r="G22" s="8">
+        <f t="shared" ref="G22:H22" si="7">(G20-G21)/G21</f>
         <v>0.94835680751173734</v>
       </c>
-      <c r="G22" s="12">
-        <f t="shared" si="6"/>
+      <c r="H22" s="12">
+        <f t="shared" si="7"/>
         <v>3.1060606060606055</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1290,72 +1427,86 @@
         <v>0.96</v>
       </c>
       <c r="E24" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="F24" s="8">
         <v>5.84</v>
       </c>
-      <c r="F24" s="8">
+      <c r="G24" s="8">
         <v>1.96</v>
       </c>
-      <c r="G24" s="12">
+      <c r="H24" s="12">
         <v>2.68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="19">
         <v>0.93</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="19">
         <v>0.95</v>
       </c>
       <c r="E25" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="F25" s="19">
         <v>6.16</v>
       </c>
-      <c r="F25" s="8">
-        <v>2.66</v>
-      </c>
-      <c r="G25" s="12">
+      <c r="G25" s="21">
+        <v>1.82</v>
+      </c>
+      <c r="H25" s="20">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="19">
         <f>(C24-C25)/C25</f>
         <v>-0.18279569892473121</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="19">
         <f>(D24-D25)/D25</f>
         <v>1.0526315789473694E-2</v>
       </c>
       <c r="E26" s="8">
-        <f t="shared" ref="E26" si="7">(E24-E25)/E25</f>
+        <f>(E24-E25)/E25</f>
+        <v>0.30158730158730152</v>
+      </c>
+      <c r="F26" s="19">
+        <f t="shared" ref="F26" si="8">(F24-F25)/F25</f>
         <v>-5.1948051948051993E-2</v>
       </c>
-      <c r="F26" s="8">
-        <f t="shared" ref="F26:G26" si="8">(F24-F25)/F25</f>
-        <v>-0.26315789473684215</v>
-      </c>
-      <c r="G26" s="12">
-        <f t="shared" si="8"/>
+      <c r="G26" s="21">
+        <f t="shared" ref="G26:H26" si="9">(G24-G25)/G25</f>
+        <v>7.6923076923076872E-2</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" si="9"/>
         <v>0.2293577981651376</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
@@ -1366,16 +1517,19 @@
         <v>1.81</v>
       </c>
       <c r="E28" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="F28" s="8">
         <v>10.63</v>
       </c>
-      <c r="F28" s="8">
+      <c r="G28" s="8">
         <v>4.0599999999999996</v>
       </c>
-      <c r="G28" s="12">
+      <c r="H28" s="12">
         <v>4.41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1386,16 +1540,19 @@
         <v>1.08</v>
       </c>
       <c r="E29" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="F29" s="8">
         <v>7.58</v>
       </c>
-      <c r="F29" s="8">
+      <c r="G29" s="8">
         <v>5.08</v>
       </c>
-      <c r="G29" s="12">
+      <c r="H29" s="12">
         <v>3.69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1408,30 +1565,35 @@
         <v>0.67592592592592582</v>
       </c>
       <c r="E30" s="8">
-        <f t="shared" ref="E30" si="9">(E28-E29)/E29</f>
+        <f>(E28-E29)/E29</f>
+        <v>0.11956521739130432</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" ref="F30" si="10">(F28-F29)/F29</f>
         <v>0.40237467018469664</v>
       </c>
-      <c r="F30" s="8">
-        <f t="shared" ref="F30:G30" si="10">(F28-F29)/F29</f>
+      <c r="G30" s="8">
+        <f t="shared" ref="G30:H30" si="11">(G28-G29)/G29</f>
         <v>-0.20078740157480324</v>
       </c>
-      <c r="G30" s="12">
-        <f t="shared" si="10"/>
+      <c r="H30" s="12">
+        <f t="shared" si="11"/>
         <v>0.19512195121951226</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="10" t="s">
         <v>1</v>
@@ -1443,146 +1605,163 @@
         <v>1.66</v>
       </c>
       <c r="E32" s="11">
+        <v>1.48</v>
+      </c>
+      <c r="F32" s="11">
         <v>7.01</v>
       </c>
-      <c r="F32" s="11">
+      <c r="G32" s="11">
         <v>6.55</v>
       </c>
-      <c r="G32" s="13">
+      <c r="H32" s="13">
         <v>1.68</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
-      <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="8"/>
-      <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="8"/>
-      <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42"/>
       <c r="D42"/>
       <c r="E42"/>
       <c r="F42"/>
       <c r="G42"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47"/>
       <c r="D47"/>
       <c r="E47"/>
       <c r="F47"/>
       <c r="G47"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H47"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="I2:L3"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="J2:M3"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C30:G30 C26:G26 C22:G22 C13:G13 C9:G9 C5:G5">
+  <conditionalFormatting sqref="C30:H30 C26:H26 C22:H22 C13:H13 C9:H9 C5:H5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-0.5"/>

</xml_diff>